<commit_message>
[Fix] Cotizaciones y Promociones
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/promotion/PromotionListado.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/promotion/PromotionListado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.Catalog\wwwroot\layout\excel\promotion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-71\source\repos\LaboratorioRamos\API\Service.Catalog\wwwroot\layout\excel\promotion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5653BD5B-34F3-468E-8411-D67584D2C0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2FBF47-1FC9-4D04-B69D-FD371D9F7358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Promociones" sheetId="1" r:id="rId1"/>
@@ -90,13 +90,13 @@
     <t>Lista</t>
   </si>
   <si>
-    <t>{{item.NombreListaPrecio}}</t>
-  </si>
-  <si>
     <t>{{item.Activo}}</t>
   </si>
   <si>
     <t>Nombre Promoción</t>
+  </si>
+  <si>
+    <t>{{item.ListaPrecio}}</t>
   </si>
 </sst>
 </file>
@@ -552,20 +552,20 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" customWidth="1"/>
-    <col min="6" max="6" width="28.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -577,12 +577,12 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -596,7 +596,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -607,13 +607,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
   </sheetData>

</xml_diff>